<commit_message>
Added Standalone functionality to the plugin
It is now possible to use the converter with CSV files and without the
rapla client itself.
</commit_message>
<xml_diff>
--- a/src/rapla_config.xlsx
+++ b/src/rapla_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\Patrick\Studium\Projektarbeiten\T3100_T3200\rapla-2-excel-plugin\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4938C859-81D4-401C-BF05-7E4D07F514FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDABC8E4-B00C-4AB5-AF1C-D876B181CDED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC461761-E902-4464-A6F0-DB3841317405}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>N+S</t>
   </si>
@@ -100,13 +100,35 @@
   </si>
   <si>
     <t>In der Zeile hier drunter kann optional ein festes Startdatum eingetragen werden. Wenn ein festes Startdatum eingetragen wird, werden die Quartals Startwochen nicht beachtet. Das Quartal beginnt in diesem Fall an dem Montag in der Woche des angegebenen Datums. In der Zeile danach kann die Abkürzung der Zeitzone angegeben werden. Standardmäßig wird, wie bei Rapla GMT verwendet.</t>
+  </si>
+  <si>
+    <t>Klausurwochentext</t>
+  </si>
+  <si>
+    <t>Hier kann ein Text mit Formatierung angegeben werden, der unterhalb der Klausurenwoche angezeigt wird.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Klausurwoche
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>! Vorläufige Termine !</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +178,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,8 +288,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -268,11 +303,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -297,6 +341,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -611,9 +661,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D276216-C963-4B1C-9A3D-58B2AD26B1FD}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -625,9 +677,10 @@
     <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="7" width="36" customWidth="1"/>
     <col min="8" max="8" width="34.5703125" customWidth="1"/>
+    <col min="9" max="9" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -652,8 +705,11 @@
       <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -678,8 +734,11 @@
       <c r="H2" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>9</v>
       </c>
@@ -699,8 +758,11 @@
         <v>6</v>
       </c>
       <c r="H3" s="21"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -713,47 +775,49 @@
       <c r="F4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="23"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="F5">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="F6">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -775,6 +839,9 @@
       <c r="A22" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I3:I5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Prints all errors or skipped lectures.
Prints all errors or skipped lectures into the stand alone GUI or the
finished frame in rapla.
</commit_message>
<xml_diff>
--- a/src/rapla_config.xlsx
+++ b/src/rapla_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\Patrick\Studium\Projektarbeiten\T3100_T3200\rapla-2-excel-plugin\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDABC8E4-B00C-4AB5-AF1C-D876B181CDED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC758F3-BADD-4ECC-A74C-B92E5B55C6D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC461761-E902-4464-A6F0-DB3841317405}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>N+S</t>
   </si>
@@ -122,6 +122,12 @@
       </rPr>
       <t>! Vorläufige Termine !</t>
     </r>
+  </si>
+  <si>
+    <t>Benutzerdefiniert</t>
+  </si>
+  <si>
+    <t>Diese Spalte wird beim Laden der Konfigruationen nicht beachtet. Die Spalte kann beliebig verwendet werden. Sie kann zum Beispiel für Gruppierungsnamen von Vorlesungen für mehr Übersichtlichkeit verwendet werden.</t>
   </si>
 </sst>
 </file>
@@ -186,7 +192,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,18 +218,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -236,12 +230,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -254,12 +242,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -267,12 +249,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,6 +268,144 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF00FF"/>
         <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -316,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -326,27 +440,44 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -661,186 +792,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D276216-C963-4B1C-9A3D-58B2AD26B1FD}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.28515625" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="36" customWidth="1"/>
-    <col min="8" max="8" width="34.5703125" customWidth="1"/>
-    <col min="9" max="9" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" customWidth="1"/>
+    <col min="10" max="10" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="13"/>
+      <c r="J3" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>15</v>
       </c>
-      <c r="I4" s="23"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="F5">
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="16"/>
+      <c r="G5">
         <v>27</v>
       </c>
-      <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="F6">
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="G6">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="20"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="23"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="24"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="25"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="26"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="27"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="28"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="29"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="30"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="31"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="32"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="33"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="34"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="35"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="36"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="37"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="38"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="39"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Copy whole font style of each lecture in the config workbook
The whole font style including the font size of the config workbook will
be copied for the lecture workbook.
</commit_message>
<xml_diff>
--- a/src/rapla_config.xlsx
+++ b/src/rapla_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\Patrick\Studium\Projektarbeiten\T3100_T3200\rapla-2-excel-plugin\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC758F3-BADD-4ECC-A74C-B92E5B55C6D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8085BFB8-9F0F-4FDC-9301-705E3653B9B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC461761-E902-4464-A6F0-DB3841317405}"/>
+    <workbookView xWindow="6240" yWindow="3360" windowWidth="21600" windowHeight="11280" xr2:uid="{DC461761-E902-4464-A6F0-DB3841317405}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="29">
   <si>
     <t>N+S</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Hier kann ein Text mit Formatierung angegeben werden, der unterhalb der Klausurenwoche angezeigt wird.</t>
+  </si>
+  <si>
+    <t>Benutzerdefiniert</t>
+  </si>
+  <si>
+    <t>Diese Spalte wird beim Laden der Konfigruationen nicht beachtet. Die Spalte kann beliebig verwendet werden. Sie kann zum Beispiel für Gruppierungsnamen von Vorlesungen für mehr Übersichtlichkeit verwendet werden.</t>
   </si>
   <si>
     <r>
@@ -115,7 +121,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -124,17 +129,27 @@
     </r>
   </si>
   <si>
-    <t>Benutzerdefiniert</t>
-  </si>
-  <si>
-    <t>Diese Spalte wird beim Laden der Konfigruationen nicht beachtet. Die Spalte kann beliebig verwendet werden. Sie kann zum Beispiel für Gruppierungsnamen von Vorlesungen für mehr Übersichtlichkeit verwendet werden.</t>
+    <r>
+      <t xml:space="preserve">Klausurwoche
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>! Vorläufige Termine !</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,9 +202,17 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="37">
@@ -447,12 +470,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
@@ -478,12 +495,24 @@
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF000000"/>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -795,7 +824,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +843,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>4</v>
@@ -846,7 +875,7 @@
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -896,8 +925,8 @@
         <v>6</v>
       </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="14" t="s">
-        <v>25</v>
+      <c r="J3" s="39" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -913,14 +942,14 @@
       <c r="G4">
         <v>15</v>
       </c>
-      <c r="J4" s="15"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="16"/>
+      <c r="B5" s="14"/>
       <c r="G5">
         <v>27</v>
       </c>
-      <c r="J5" s="15"/>
+      <c r="J5" s="40"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
@@ -932,88 +961,88 @@
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
+      <c r="B10" s="16"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
+      <c r="B11" s="17"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
+      <c r="B12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
+      <c r="B13" s="19"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
+      <c r="B14" s="20"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
+      <c r="B16" s="21"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
+      <c r="B18" s="22"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
+      <c r="B19" s="23"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
+      <c r="B20" s="24"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="27"/>
+      <c r="B21" s="25"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="28"/>
+      <c r="B22" s="26"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="29"/>
+      <c r="B23" s="27"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="30"/>
+      <c r="B24" s="28"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
+      <c r="B26" s="29"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="32"/>
+      <c r="B27" s="30"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="33"/>
+      <c r="B28" s="31"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="34"/>
+      <c r="B29" s="32"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="35"/>
+      <c r="B30" s="33"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="36"/>
+      <c r="B31" s="34"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="37"/>
+      <c r="B32" s="35"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="38"/>
+      <c r="B33" s="36"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="39"/>
+      <c r="B34" s="37"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="40"/>
+      <c r="B35" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add fonts from config workbook to whole cell
</commit_message>
<xml_diff>
--- a/src/rapla_config.xlsx
+++ b/src/rapla_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\Patrick\Studium\Projektarbeiten\T3100_T3200\rapla-2-excel-plugin\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8085BFB8-9F0F-4FDC-9301-705E3653B9B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A577D83-A571-4B96-833C-5B651A658FD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6240" yWindow="3360" windowWidth="21600" windowHeight="11280" xr2:uid="{DC461761-E902-4464-A6F0-DB3841317405}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>N+S</t>
   </si>
@@ -121,6 +121,7 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -128,28 +129,12 @@
       <t>! Vorläufige Termine !</t>
     </r>
   </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Klausurwoche
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>! Vorläufige Termine !</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,20 +166,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,14 +174,14 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -453,53 +425,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,6 +482,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF595959"/>
       <color rgb="FF000000"/>
       <color rgb="FFFF00FF"/>
     </mruColors>
@@ -824,13 +798,13 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.42578125" style="38" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="37.42578125" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="42.7109375" customWidth="1" collapsed="1"/>
@@ -841,72 +815,72 @@
     <col min="10" max="10" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" s="41" customFormat="1" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="41" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -924,13 +898,13 @@
       <c r="H3">
         <v>6</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -945,104 +919,104 @@
       <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
+      <c r="B5" s="7"/>
       <c r="G5">
         <v>27</v>
       </c>
       <c r="J5" s="40"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
+      <c r="B6" s="8"/>
       <c r="G6">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
+      <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
+      <c r="B10" s="12"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
+      <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
+      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
+      <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
+      <c r="B14" s="16"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
+      <c r="B15" s="17"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
+      <c r="B16" s="18"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
+      <c r="B17" s="19"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
+      <c r="B18" s="20"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="23"/>
+      <c r="B19" s="21"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
+      <c r="B20" s="22"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
+      <c r="B21" s="23"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
+      <c r="B22" s="24"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="27"/>
+      <c r="B23" s="25"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="28"/>
+      <c r="B24" s="26"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
+      <c r="B25" s="27"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="29"/>
+      <c r="B26" s="28"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="30"/>
+      <c r="B27" s="29"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="31"/>
+      <c r="B28" s="30"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="32"/>
+      <c r="B29" s="31"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="33"/>
+      <c r="B30" s="32"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="34"/>
+      <c r="B31" s="33"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="35"/>
+      <c r="B32" s="34"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="36"/>
+      <c r="B33" s="35"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="37"/>
+      <c r="B34" s="36"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="38"/>
+      <c r="B35" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fixed bug with wrong font creation and color copying
Added all created fonts to the lecture workbook and replaced the
deprecated getter and setter method for indexed colors for a font with
the getter and setter method for xssfcolors for the font.
</commit_message>
<xml_diff>
--- a/src/rapla_config.xlsx
+++ b/src/rapla_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\Patrick\Studium\Projektarbeiten\T3100_T3200\rapla-2-excel-plugin\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A577D83-A571-4B96-833C-5B651A658FD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4118A73-E430-4653-B99F-7CFAD46E7F28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="3360" windowWidth="21600" windowHeight="11280" xr2:uid="{DC461761-E902-4464-A6F0-DB3841317405}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC461761-E902-4464-A6F0-DB3841317405}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -165,13 +165,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
@@ -182,6 +175,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,42 +438,42 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -798,13 +798,13 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" style="38" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.42578125" style="23" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="37.42578125" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="42.7109375" customWidth="1" collapsed="1"/>
@@ -847,35 +847,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="41" customFormat="1" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+    <row r="2" spans="1:10" s="24" customFormat="1" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -899,7 +899,7 @@
         <v>6</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="25" t="s">
         <v>27</v>
       </c>
     </row>
@@ -916,14 +916,14 @@
       <c r="G4">
         <v>15</v>
       </c>
-      <c r="J4" s="40"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="G5">
         <v>27</v>
       </c>
-      <c r="J5" s="40"/>
+      <c r="J5" s="26"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
@@ -941,82 +941,82 @@
       <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
+      <c r="B10" s="27"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
+      <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
+      <c r="B12" s="29"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="12"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
+      <c r="B14" s="13"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
+      <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
+      <c r="B16" s="30"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
+      <c r="B17" s="32"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
+      <c r="B18" s="31"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
+      <c r="B19" s="33"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
+      <c r="B20" s="35"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="23"/>
+      <c r="B21" s="34"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="24"/>
+      <c r="B22" s="36"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
+      <c r="B23" s="37"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="26"/>
+      <c r="B24" s="38"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
+      <c r="B25" s="15"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
+      <c r="B26" s="16"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="29"/>
+      <c r="B27" s="17"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="30"/>
+      <c r="B28" s="39"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="31"/>
+      <c r="B29" s="41"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="32"/>
+      <c r="B30" s="40"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="33"/>
+      <c r="B31" s="18"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="34"/>
+      <c r="B32" s="19"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="35"/>
+      <c r="B33" s="20"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="36"/>
+      <c r="B34" s="21"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="37"/>
+      <c r="B35" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>